<commit_message>
adding FRPT to company info
</commit_message>
<xml_diff>
--- a/company_Info /Company_Info.xlsx
+++ b/company_Info /Company_Info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssadavis/Documents/Bootcamp/Modules/20/Alyssa/Visualization_Mockups/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssadavis/Documents/Bootcamp/Modules/20/Final_Project/company_Info /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E76319-E533-3B44-A839-65BB901D3E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33246E04-2146-0A41-85D8-6BE44FEC3A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{3E001325-A366-324F-B3E8-123F9EECBCE1}"/>
+    <workbookView xWindow="-27160" yWindow="3780" windowWidth="28800" windowHeight="17500" xr2:uid="{3E001325-A366-324F-B3E8-123F9EECBCE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,23 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Company</t>
   </si>
   <si>
-    <t>Stock Ticker</t>
-  </si>
-  <si>
-    <t>Date IPO</t>
-  </si>
-  <si>
-    <t>Pet Market Segment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Company Size </t>
-  </si>
-  <si>
     <t>CHWY</t>
   </si>
   <si>
@@ -62,9 +50,6 @@
     <t>Pet Supplies, E-commerce</t>
   </si>
   <si>
-    <t>Market Capitalization</t>
-  </si>
-  <si>
     <t>13.95B</t>
   </si>
   <si>
@@ -108,6 +93,33 @@
   </si>
   <si>
     <t>438.348M</t>
+  </si>
+  <si>
+    <t>FRPT</t>
+  </si>
+  <si>
+    <t>Stock_Ticker</t>
+  </si>
+  <si>
+    <t>Date_IPO</t>
+  </si>
+  <si>
+    <t>Market_Capitalization</t>
+  </si>
+  <si>
+    <t>Pet_Market_Segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company_Size </t>
+  </si>
+  <si>
+    <t>Freshpet, Inc.</t>
+  </si>
+  <si>
+    <t>2.582B</t>
+  </si>
+  <si>
+    <t>Pet Food</t>
   </si>
 </sst>
 </file>
@@ -470,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CCB191-A312-9349-8AF8-122041386E6B}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,39 +500,39 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3">
         <v>43630</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1">
         <v>21300</v>
@@ -528,19 +540,19 @@
     </row>
     <row r="3" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3">
         <v>43363</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1">
         <v>10200</v>
@@ -548,19 +560,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="3">
         <v>42936</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>849</v>
@@ -568,19 +580,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3">
         <v>33410</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1">
         <v>10000</v>
@@ -588,22 +600,42 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3">
         <v>43862</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1">
         <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3">
+        <v>41944</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1">
+        <v>789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>